<commit_message>
fix: esm bin bug
</commit_message>
<xml_diff>
--- a/test/data/empty-data-row-test-input.xlsx
+++ b/test/data/empty-data-row-test-input.xlsx
@@ -56,9 +56,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -191,7 +191,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -207,9 +207,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -217,9 +214,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -232,9 +226,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1319,14 +1310,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1339,206 +1330,37 @@
       <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
     </row>
     <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" t="s" s="8">
+      <c r="B2" s="6"/>
+      <c r="C2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>2</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="13">
+      <c r="B4" t="s" s="11">
         <v>6</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="C4" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
fix: esm bin bug (#107)
fix: esm bin bug

fix: empty cell missing bug
</commit_message>
<xml_diff>
--- a/test/data/empty-data-row-test-input.xlsx
+++ b/test/data/empty-data-row-test-input.xlsx
@@ -56,9 +56,9 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -191,7 +191,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -207,9 +207,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -217,9 +214,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -232,9 +226,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1319,14 +1310,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1339,206 +1330,37 @@
       <c r="C1" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
     </row>
     <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="A2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" t="s" s="8">
+      <c r="B2" s="6"/>
+      <c r="C2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>2</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="A4" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="13">
+      <c r="B4" t="s" s="11">
         <v>6</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="C4" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="14"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="14"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="14"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>